<commit_message>
feat: fix die hard again
</commit_message>
<xml_diff>
--- a/source/en/talent_die_hard.xlsx
+++ b/source/en/talent_die_hard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Tipo</t>
   </si>
@@ -61,9 +61,6 @@
     <t>You gain the following benefits:</t>
   </si>
   <si>
-    <t>Increase your Constitution score by 1, to a maximum of 20.</t>
-  </si>
-  <si>
     <t>You have advantage in Death Saving Throws.</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
   </si>
   <si>
     <t>Abilità da aumentare</t>
-  </si>
-  <si>
-    <t>con|str</t>
   </si>
   <si>
     <t>con</t>
@@ -542,31 +536,25 @@
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="6"/>
       <c r="E7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="8"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9">
       <c r="A9" s="2"/>
@@ -576,11 +564,11 @@
       <c r="E9" s="8"/>
     </row>
     <row r="10">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11">
       <c r="A11" s="6"/>
@@ -7511,13 +7499,6 @@
       <c r="C1000" s="7"/>
       <c r="D1000" s="6"/>
       <c r="E1000" s="7"/>
-    </row>
-    <row r="1001">
-      <c r="A1001" s="6"/>
-      <c r="B1001" s="6"/>
-      <c r="C1001" s="7"/>
-      <c r="D1001" s="6"/>
-      <c r="E1001" s="7"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -7540,13 +7521,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -11590,34 +11571,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1">
         <v>1.0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: die hard again
</commit_message>
<xml_diff>
--- a/source/en/talent_die_hard.xlsx
+++ b/source/en/talent_die_hard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Tipo</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>You gain the following benefits:</t>
-  </si>
-  <si>
-    <t>Increase your Constitution score by 1, to a maximum of 20.</t>
   </si>
   <si>
     <t>You have advantage in Death Saving Throws.</t>
@@ -539,31 +536,25 @@
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="6"/>
       <c r="E7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="8"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9">
       <c r="A9" s="2"/>
@@ -573,11 +564,11 @@
       <c r="E9" s="8"/>
     </row>
     <row r="10">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11">
       <c r="A11" s="6"/>
@@ -7508,13 +7499,6 @@
       <c r="C1000" s="7"/>
       <c r="D1000" s="6"/>
       <c r="E1000" s="7"/>
-    </row>
-    <row r="1001">
-      <c r="A1001" s="6"/>
-      <c r="B1001" s="6"/>
-      <c r="C1001" s="7"/>
-      <c r="D1001" s="6"/>
-      <c r="E1001" s="7"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -7537,13 +7521,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -11587,21 +11571,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1">
         <v>1.0</v>

</xml_diff>